<commit_message>
Auro-write process for all forms
</commit_message>
<xml_diff>
--- a/penyata-akaun-hr-2022.xlsx
+++ b/penyata-akaun-hr-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suriati binti Jaafar\Documents\projek-penyata-hr\utama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ABB8EB-22C4-43EC-8C89-6B015D6AB831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401634B0-DB64-477A-B2E3-560633E6E44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -156,11 +156,6 @@
     <font>
       <sz val="25"/>
       <color theme="1"/>
-      <name val="Impact"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Impact"/>
     </font>
     <font>
@@ -226,6 +221,19 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Impact"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -488,27 +496,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -516,34 +524,35 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,8 +813,8 @@
   </sheetPr>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -835,18 +844,18 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="12.5">
       <c r="A4" s="4"/>
-      <c r="C4" s="29"/>
-      <c r="E4" s="33" t="s">
+      <c r="C4" s="33"/>
+      <c r="E4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
@@ -862,23 +871,23 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="34"/>
-      <c r="D7" s="27"/>
+      <c r="D7" s="29"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="13">
       <c r="A8" s="4"/>
       <c r="B8" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="36"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="13">
       <c r="A9" s="4"/>
       <c r="B9" s="37" t="s">
         <v>6</v>
@@ -897,7 +906,7 @@
     </row>
     <row r="12" spans="1:7" ht="13">
       <c r="A12" s="4"/>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="9"/>
@@ -907,27 +916,27 @@
     </row>
     <row r="13" spans="1:7" ht="13">
       <c r="A13" s="4"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="13">
       <c r="A14" s="4"/>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="12">
         <v>500</v>
       </c>
@@ -939,10 +948,10 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -993,7 +1002,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="13">
       <c r="A19" s="4"/>
       <c r="B19" s="30"/>
       <c r="C19" s="31"/>
@@ -1007,10 +1016,10 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -1065,10 +1074,10 @@
     </row>
     <row r="25" spans="1:7" ht="12.5">
       <c r="A25" s="4"/>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1137,17 +1146,17 @@
       <c r="D30" s="31"/>
       <c r="E30" s="32"/>
       <c r="F30" s="18">
-        <f>D27-E27+D28-E28+D29-E29-E26</f>
+        <f>D27-E27+D28-E28+D29-E29-E26+D26</f>
         <v>2600</v>
       </c>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" ht="12.5">
       <c r="A31" s="4"/>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="27"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -1287,24 +1296,24 @@
     </row>
     <row r="42" spans="1:7" ht="17.5">
       <c r="A42" s="4"/>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
       <c r="G42" s="6"/>
     </row>
     <row r="43" spans="1:7" ht="17.5">
       <c r="A43" s="4"/>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
       <c r="G43" s="6"/>
     </row>
     <row r="44" spans="1:7" ht="12.5">
@@ -1318,6 +1327,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="E4:F4"/>
@@ -1328,13 +1344,6 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B39:E39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Standardized the Formatting for Data in Excel
</commit_message>
<xml_diff>
--- a/penyata-akaun-hr-2022.xlsx
+++ b/penyata-akaun-hr-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suriati binti Jaafar\Documents\projek-penyata-hr\utama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\penyata-sesi-hr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401634B0-DB64-477A-B2E3-560633E6E44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590F960E-3D02-4BB2-9B73-2AC6641955E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>UNIT PEMBANGUNAN</t>
   </si>
@@ -74,12 +72,6 @@
     <t>Kali Kedua</t>
   </si>
   <si>
-    <t>Kali Ketiga &amp; Keempat</t>
-  </si>
-  <si>
-    <t>JPPM/ JDM/ JDRM</t>
-  </si>
-  <si>
     <t>Kali Ketiga</t>
   </si>
   <si>
@@ -129,13 +121,16 @@
   </si>
   <si>
     <t>Description / Deskripsi</t>
+  </si>
+  <si>
+    <t>JPPM / JDM / JDRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -227,16 +222,23 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Impact"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Impact"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -487,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -534,10 +536,13 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -546,13 +551,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,19 +813,19 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -844,18 +846,18 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="12.5">
+    <row r="4" spans="1:7" ht="14.25">
       <c r="A4" s="4"/>
-      <c r="C4" s="33"/>
-      <c r="E4" s="43" t="s">
+      <c r="C4" s="31"/>
+      <c r="E4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="44"/>
+      <c r="F4" s="43"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
@@ -874,26 +876,26 @@
       <c r="B7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="29"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="13">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="4"/>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="36"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="37"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="13">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="4"/>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
@@ -904,39 +906,39 @@
       <c r="A11" s="4"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="13">
+    <row r="12" spans="1:7" ht="12.75">
       <c r="A12" s="4"/>
       <c r="B12" s="26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="13">
+    <row r="13" spans="1:7" ht="12.75">
       <c r="A13" s="4"/>
-      <c r="B13" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="39"/>
+      <c r="B13" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="40"/>
       <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="13">
+    <row r="14" spans="1:7" ht="12.75">
       <c r="A14" s="4"/>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="12">
         <v>500</v>
       </c>
@@ -964,10 +966,10 @@
         <v>11</v>
       </c>
       <c r="D16" s="15">
-        <v>3200</v>
+        <v>250</v>
       </c>
       <c r="E16" s="16">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="6"/>
@@ -979,10 +981,10 @@
         <v>12</v>
       </c>
       <c r="D17" s="17">
-        <v>5300</v>
+        <v>500</v>
       </c>
       <c r="E17" s="12">
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="6"/>
@@ -994,7 +996,7 @@
         <v>13</v>
       </c>
       <c r="D18" s="17">
-        <v>1765</v>
+        <v>750</v>
       </c>
       <c r="E18" s="12">
         <v>750</v>
@@ -1002,341 +1004,365 @@
       <c r="F18" s="12"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="13">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="4"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="18">
-        <f>D16-E16+D17-E17+D18-E18</f>
-        <v>8555</v>
-      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1000</v>
+      </c>
+      <c r="F19" s="12"/>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="12.75">
       <c r="A20" s="4"/>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="18">
+        <f>D16-E16+D17-E17+D18-E18+D19-E19+F14</f>
+        <v>500</v>
+      </c>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="12.5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="12">
-        <v>1000</v>
-      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="12.5">
+    <row r="22" spans="1:7" ht="12.75">
       <c r="A22" s="4"/>
       <c r="B22" s="11"/>
       <c r="C22" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="D22" s="17"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="12.5">
+    <row r="23" spans="1:7" ht="12.75">
       <c r="A23" s="4"/>
       <c r="B23" s="11"/>
       <c r="C23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="D23" s="17">
+        <v>250</v>
+      </c>
+      <c r="E23" s="12">
+        <v>250</v>
+      </c>
       <c r="F23" s="12"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="13">
+    <row r="24" spans="1:7" ht="12.75">
       <c r="A24" s="4"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="18">
-        <f>-E21-E22-E23</f>
-        <v>-1000</v>
-      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="17">
+        <v>500</v>
+      </c>
+      <c r="E24" s="12">
+        <v>500</v>
+      </c>
+      <c r="F24" s="12"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="12.5">
+    <row r="25" spans="1:7" ht="12.75">
       <c r="A25" s="4"/>
-      <c r="B25" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="17">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1000</v>
+      </c>
       <c r="F25" s="12"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="12.5">
+    <row r="26" spans="1:7" ht="12.75">
       <c r="A26" s="4"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="18">
+        <f>D23-E23+D24-E24+D25-E25-E22+D22</f>
+        <v>0</v>
+      </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="12.5">
+    <row r="27" spans="1:7" ht="12.75">
       <c r="A27" s="4"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="17">
-        <v>200</v>
-      </c>
-      <c r="E27" s="12">
-        <v>200</v>
-      </c>
+      <c r="B27" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="12.5">
+    <row r="28" spans="1:7" ht="12.75">
       <c r="A28" s="4"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="17">
-        <v>600</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="12">
-        <v>1400</v>
+        <v>250</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="12.5">
+    <row r="29" spans="1:7" ht="12.75">
       <c r="A29" s="4"/>
       <c r="B29" s="11"/>
       <c r="C29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="17">
-        <v>3800</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D29" s="20"/>
       <c r="E29" s="12">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" ht="13">
+    <row r="30" spans="1:7" ht="12.75">
       <c r="A30" s="4"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="18">
-        <f>D27-E27+D28-E28+D29-E29-E26+D26</f>
-        <v>2600</v>
-      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="12">
+        <v>750</v>
+      </c>
+      <c r="F30" s="12"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" ht="12.5">
+    <row r="31" spans="1:7" ht="12.75">
       <c r="A31" s="4"/>
-      <c r="B31" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="12">
+        <v>1000</v>
+      </c>
       <c r="F31" s="12"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" ht="12.5">
+    <row r="32" spans="1:7" ht="12.75">
       <c r="A32" s="4"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="17">
-        <v>400</v>
-      </c>
-      <c r="E32" s="12">
-        <v>0</v>
-      </c>
-      <c r="F32" s="12"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="18">
+        <f>-E28-E29-E30-E31</f>
+        <v>-2500</v>
+      </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="12.5">
+    <row r="33" spans="1:7" ht="12.75">
       <c r="A33" s="4"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="17">
-        <v>0</v>
-      </c>
-      <c r="E33" s="12">
-        <v>300</v>
-      </c>
+      <c r="B33" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="12.5">
+    <row r="34" spans="1:7" ht="12.75">
       <c r="A34" s="4"/>
       <c r="B34" s="11"/>
       <c r="C34" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D34" s="17">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E34" s="12">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F34" s="12"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" ht="12.5">
+    <row r="35" spans="1:7" ht="12.75">
       <c r="A35" s="4"/>
       <c r="B35" s="11"/>
       <c r="C35" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D35" s="17">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E35" s="12">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" ht="12.5">
+    <row r="36" spans="1:7" ht="12.75">
       <c r="A36" s="4"/>
       <c r="B36" s="11"/>
       <c r="C36" s="14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D36" s="17">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E36" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F36" s="12"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="12.5">
+    <row r="37" spans="1:7" ht="12.75">
       <c r="A37" s="4"/>
       <c r="B37" s="11"/>
       <c r="C37" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D37" s="17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E37" s="12">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" ht="12.5">
+    <row r="38" spans="1:7" ht="12.75">
       <c r="A38" s="4"/>
       <c r="B38" s="11"/>
       <c r="C38" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="14">
-        <v>0</v>
-      </c>
-      <c r="E38" s="21">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D38" s="17">
+        <v>200</v>
+      </c>
+      <c r="E38" s="12">
+        <v>200</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" ht="13">
+    <row r="39" spans="1:7" ht="12.75">
       <c r="A39" s="4"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="18">
-        <f>D32-E32+D33-E33+D34-E34+D35-E35+D36-E36+D37-E37+D38-E38</f>
-        <v>1100</v>
-      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="17">
+        <v>200</v>
+      </c>
+      <c r="E39" s="12">
+        <v>200</v>
+      </c>
+      <c r="F39" s="12"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="15.5">
+    <row r="40" spans="1:7" ht="12.75">
       <c r="A40" s="4"/>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="11"/>
+      <c r="C40" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="14">
+        <v>100</v>
+      </c>
+      <c r="E40" s="21">
+        <v>100</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" ht="12.75">
+      <c r="A41" s="4"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="18">
+        <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D40-E40</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4"/>
+      <c r="B42" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="22">
+        <f>F20+F32+F26+F41</f>
+        <v>-2000</v>
+      </c>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" ht="12.75">
+      <c r="A43" s="4"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75">
+      <c r="A44" s="4"/>
+      <c r="B44" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.75">
+      <c r="A45" s="4"/>
+      <c r="B45" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="22">
-        <f>F14+F19+F24+F30+F39</f>
-        <v>11755</v>
-      </c>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="12.5">
-      <c r="A41" s="4"/>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="17.5">
-      <c r="A42" s="4"/>
-      <c r="B42" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" ht="17.5">
-      <c r="A43" s="4"/>
-      <c r="B43" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" ht="12.5">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" ht="12.75">
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="E4:F4"/>
+  <mergeCells count="16">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
@@ -1344,6 +1370,13 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B41:E41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
New penyata template format
</commit_message>
<xml_diff>
--- a/penyata-akaun-hr-2022.xlsx
+++ b/penyata-akaun-hr-2022.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>UNIT PEMBANGUNAN</t>
   </si>
@@ -81,16 +81,7 @@
     <t>Penyertaan Pertandingan</t>
   </si>
   <si>
-    <t>Kolokium Homeroom</t>
-  </si>
-  <si>
-    <t>Hari Bumi</t>
-  </si>
-  <si>
-    <t>Dokumentasi Kreatif</t>
-  </si>
-  <si>
-    <t>Menulis Cerpen</t>
+    <t>Nama Pertandingan</t>
   </si>
   <si>
     <t>CLOSING BALANCE FOR YEAR 2022 / BAKI PENUTUP TAHUN 2022</t>
@@ -396,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -432,10 +423,16 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment horizontal="right" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf borderId="17" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="18" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -852,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="28">
-        <v>3200.0</v>
+        <v>0.0</v>
       </c>
       <c r="E16" s="29">
-        <v>500.0</v>
+        <v>0.0</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="6"/>
@@ -867,10 +864,10 @@
         <v>15</v>
       </c>
       <c r="D17" s="28">
-        <v>5300.0</v>
-      </c>
-      <c r="E17" s="25">
-        <v>460.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.0</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="6"/>
@@ -881,7 +878,7 @@
       <c r="C18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="31">
         <v>0.0</v>
       </c>
       <c r="E18" s="25">
@@ -897,23 +894,23 @@
         <v>17</v>
       </c>
       <c r="D19" s="28">
-        <v>1765.0</v>
-      </c>
-      <c r="E19" s="25">
-        <v>750.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E19" s="30">
+        <v>0.0</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="4"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35">
         <f>D16-E16+D17-E17+D18-E18+D19-E19+F14</f>
-        <v>9055</v>
+        <v>500</v>
       </c>
       <c r="G20" s="6"/>
     </row>
@@ -934,7 +931,7 @@
       <c r="C22" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="31">
         <v>0.0</v>
       </c>
       <c r="E22" s="25">
@@ -950,10 +947,10 @@
         <v>15</v>
       </c>
       <c r="D23" s="28">
-        <v>200.0</v>
-      </c>
-      <c r="E23" s="25">
-        <v>200.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0.0</v>
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="6"/>
@@ -965,10 +962,10 @@
         <v>16</v>
       </c>
       <c r="D24" s="28">
-        <v>600.0</v>
-      </c>
-      <c r="E24" s="25">
-        <v>1400.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0.0</v>
       </c>
       <c r="F24" s="25"/>
       <c r="G24" s="6"/>
@@ -980,23 +977,23 @@
         <v>17</v>
       </c>
       <c r="D25" s="28">
-        <v>3800.0</v>
-      </c>
-      <c r="E25" s="25">
-        <v>400.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0.0</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="4"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33">
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35">
         <f>D23-E23+D24-E24+D25-E25-E22+D22</f>
-        <v>2600</v>
+        <v>0</v>
       </c>
       <c r="G26" s="6"/>
     </row>
@@ -1014,10 +1011,10 @@
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="35"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="25">
         <v>0.0</v>
       </c>
@@ -1030,7 +1027,7 @@
       <c r="C29" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="35"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="25">
         <v>0.0</v>
       </c>
@@ -1043,7 +1040,7 @@
       <c r="C30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="35"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="25">
         <v>0.0</v>
       </c>
@@ -1056,7 +1053,7 @@
       <c r="C31" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="25">
         <v>0.0</v>
       </c>
@@ -1065,11 +1062,11 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="4"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35">
         <f>-E28-E29-E30-E31</f>
         <v>0</v>
       </c>
@@ -1089,11 +1086,11 @@
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="4"/>
       <c r="B34" s="24"/>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="38" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="28">
-        <v>400.0</v>
+        <v>0.0</v>
       </c>
       <c r="E34" s="25">
         <v>0.0</v>
@@ -1104,14 +1101,14 @@
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="28">
-        <v>0.0</v>
-      </c>
-      <c r="E35" s="25">
-        <v>300.0</v>
+      <c r="C35" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="E35" s="30">
+        <v>0.0</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="6"/>
@@ -1119,11 +1116,11 @@
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="4"/>
       <c r="B36" s="24"/>
-      <c r="C36" s="36" t="s">
-        <v>23</v>
+      <c r="C36" s="38" t="s">
+        <v>21</v>
       </c>
       <c r="D36" s="28">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="E36" s="25">
         <v>0.0</v>
@@ -1134,10 +1131,10 @@
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" s="24"/>
-      <c r="C37" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="28">
+      <c r="C37" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="31">
         <v>0.0</v>
       </c>
       <c r="E37" s="25">
@@ -1149,8 +1146,10 @@
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="4"/>
       <c r="B38" s="24"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28">
+      <c r="C38" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="31">
         <v>0.0</v>
       </c>
       <c r="E38" s="25">
@@ -1162,8 +1161,10 @@
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="4"/>
       <c r="B39" s="24"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="28">
+      <c r="C39" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="31">
         <v>0.0</v>
       </c>
       <c r="E39" s="25">
@@ -1175,11 +1176,13 @@
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="4"/>
       <c r="B40" s="24"/>
-      <c r="C40" s="27"/>
+      <c r="C40" s="38" t="s">
+        <v>21</v>
+      </c>
       <c r="D40" s="27">
         <v>0.0</v>
       </c>
-      <c r="E40" s="37">
+      <c r="E40" s="39">
         <v>0.0</v>
       </c>
       <c r="F40" s="25"/>
@@ -1187,24 +1190,24 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="4"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33">
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="35">
         <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D40-E40</f>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="G41" s="6"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4"/>
-      <c r="B42" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="39">
+      <c r="B42" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="41">
         <f>F20+F32+F26+F41</f>
-        <v>12755</v>
+        <v>500</v>
       </c>
       <c r="G42" s="6"/>
     </row>
@@ -1214,26 +1217,26 @@
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" s="4"/>
-      <c r="B44" s="40" t="s">
-        <v>26</v>
+      <c r="B44" s="42" t="s">
+        <v>23</v>
       </c>
       <c r="G44" s="6"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="40" t="s">
-        <v>27</v>
+      <c r="B45" s="42" t="s">
+        <v>24</v>
       </c>
       <c r="G45" s="6"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="41"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="43"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
     </row>
     <row r="47" ht="15.75" customHeight="1"/>
     <row r="48" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fix where 'Nama Pertandingan' appears in penyata
</commit_message>
<xml_diff>
--- a/penyata-akaun-hr-2022.xlsx
+++ b/penyata-akaun-hr-2022.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="5uTpFTdiHFrvmmxzSO75uQhA1gHqMeDZvpPr8Hz72Ng="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="wj8x6CjY4NsIt3w57xikKLRVoEmiCPXjJglSqeUH9Io="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>UNIT PEMBANGUNAN</t>
   </si>
@@ -387,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -445,6 +445,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1179,7 +1182,7 @@
       <c r="C40" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="27">
+      <c r="D40" s="38">
         <v>0.0</v>
       </c>
       <c r="E40" s="39">
@@ -1190,55 +1193,69 @@
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="4"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="35">
-        <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D40-E40</f>
+      <c r="B41" s="24"/>
+      <c r="C41" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="E41" s="40">
+        <v>0.0</v>
+      </c>
+      <c r="F41" s="25"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" ht="12.75" customHeight="1">
+      <c r="A42" s="4"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="35">
+        <f>D34-E34+D35-E35+D36-E36+D37-E37+D38-E38+D39-E39+D41-E41+D40-E40</f>
         <v>0</v>
       </c>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="4"/>
-      <c r="B42" s="40" t="s">
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="4"/>
+      <c r="B43" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="41">
-        <f>F20+F32+F26+F41</f>
+      <c r="F43" s="42">
+        <f>F20+F32+F26+F42</f>
         <v>500</v>
       </c>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="4"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" ht="18.75" customHeight="1">
+    <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="4"/>
-      <c r="B44" s="42" t="s">
-        <v>23</v>
-      </c>
       <c r="G44" s="6"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" ht="18.75" customHeight="1">
+      <c r="A46" s="4"/>
+      <c r="B46" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="43"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-    </row>
-    <row r="47" ht="15.75" customHeight="1"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" ht="12.75" customHeight="1">
+      <c r="A47" s="44"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
+    </row>
     <row r="48" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
@@ -2192,6 +2209,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="C3:C4"/>
@@ -2201,15 +2219,15 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B44:F44"/>
     <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>